<commit_message>
Working on employee binder GH-305
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -26,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,11 +48,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Портретное</t>
+          <t xml:space="preserve">В портретной ориентации</t>
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0">
+    <comment ref="A34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A39" authorId="0">
+    <comment ref="A40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -83,105 +83,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
   <si>
     <t xml:space="preserve">Общие</t>
   </si>
   <si>
-    <t xml:space="preserve">Фамилия</t>
+    <t xml:space="preserve">Фамилия:</t>
   </si>
   <si>
     <t xml:space="preserve">{{LastName}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Имя</t>
+    <t xml:space="preserve">Имя:</t>
   </si>
   <si>
     <t xml:space="preserve">{{FirstName}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Отчество</t>
+    <t xml:space="preserve">Отчество:</t>
   </si>
   <si>
     <t xml:space="preserve">{{OtherName}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Фото (URL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Альтернативное фото (URL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Пользователь сайта (email/имя входа)</t>
+    <t xml:space="preserve">Фото</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фото (URL):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{PhotoUrl}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Альтернативное фото (URL):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{AltPhotoUrl}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Контакты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Телефон:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{Phone}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сотовый:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{CellPhone}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Факс:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{Fax}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Электронная почта:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{Email}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дополнительная электронная почта:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{SecondaryEmail}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Имя входа/email на volgau.com:</t>
   </si>
   <si>
     <t xml:space="preserve">{{UserName}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Контакты</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Телефон</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{Phone}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сотовый</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{CellPhone}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Факс</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{Fax}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Эл. почта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{Email}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Доп. эл. Почта</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{SecondaryEmail}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Личный веб-сайт</t>
+    <t xml:space="preserve">Личный веб-сайт:</t>
   </si>
   <si>
     <t xml:space="preserve">{{WebSite}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Метка веб-сайта</t>
+    <t xml:space="preserve">Текстовая метка веб-сайта:</t>
   </si>
   <si>
     <t xml:space="preserve">{{WebSiteLabel}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Клиент мновенных сообщений</t>
+    <t xml:space="preserve">Клиент мновенных сообщений:</t>
   </si>
   <si>
     <t xml:space="preserve">{{Messenger}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Author ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{AuthorID}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рабочее место</t>
+    <t xml:space="preserve">Author ID на eLibrary.ru:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ScienceIndexAuthorId}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Или ссылка на eLibrary.ru:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.elibrary.ru/author_items.asp?authorid={{ScienceIndexAuthorId}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рабочее место:</t>
   </si>
   <si>
     <t xml:space="preserve">{{WorkingPlace}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Рабочий график</t>
+    <t xml:space="preserve">Рабочий график:</t>
   </si>
   <si>
     <t xml:space="preserve">{{WorkSchedule}}</t>
@@ -190,16 +205,16 @@
     <t xml:space="preserve">Стаж работы</t>
   </si>
   <si>
-    <t xml:space="preserve">Общий стаж (лет)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{Experience}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Стаж по специальности (лет)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{ExperienceBySpec}}</t>
+    <t xml:space="preserve">Общий стаж (лет):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ExperienceYears}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Стаж по специальности (лет):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ExperienceYearsBySpec}}</t>
   </si>
   <si>
     <t xml:space="preserve">Должности</t>
@@ -217,13 +232,13 @@
     <t xml:space="preserve">{% for position in Positions %}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{position.Title}}</t>
+    <t xml:space="preserve">{{position.PositionTitle}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{position.DivisionTitle}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{position.IsPrimary}}</t>
+    <t xml:space="preserve">{{position.IsPrime}}</t>
   </si>
   <si>
     <t xml:space="preserve">{% endfor %}</t>
@@ -262,7 +277,7 @@
     <t xml:space="preserve">{{education.Title}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{education.Level}}</t>
+    <t xml:space="preserve">{{education.TitleSuffix}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{education.Description}}</t>
@@ -301,6 +316,9 @@
     <t xml:space="preserve">Наименование (краткое)</t>
   </si>
   <si>
+    <t xml:space="preserve">Дополнение наименования</t>
+  </si>
+  <si>
     <t xml:space="preserve">Титульное (да/нет)</t>
   </si>
   <si>
@@ -316,6 +334,9 @@
     <t xml:space="preserve">{{achievement.Title}}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{achievement.TitleSuffix}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{achievement.IsTitle}}</t>
   </si>
   <si>
@@ -328,7 +349,7 @@
     <t xml:space="preserve">Дисциплины</t>
   </si>
   <si>
-    <t xml:space="preserve">Обр. Программа</t>
+    <t xml:space="preserve">Образовательная программа</t>
   </si>
   <si>
     <t xml:space="preserve">Профиль обр. программы</t>
@@ -343,10 +364,10 @@
     <t xml:space="preserve">{{discipline.EduProgram}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{discipline.EduProfile}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{Discipline.EduLevel}}</t>
+    <t xml:space="preserve">{{discipline.EduProgramProfile}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{discipline.EduLevel}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{discipline.Disciplines}}</t>
@@ -555,7 +576,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -570,6 +591,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -589,10 +614,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -600,10 +625,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="53.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="71.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="71.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,416 +662,446 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="B25" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>46</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C30" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="1" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="1" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="1" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="F40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="G40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="0" t="s">
         <v>69</v>
       </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="F42" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="A43" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>83</v>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>88</v>
-      </c>
+      <c r="A53" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="F53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" s="3"/>
-    </row>
-    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>90</v>
+      <c r="A54" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1079,112 +1135,112 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extract class, add service information sheet GH-305
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Сведения о сотруднике" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Инструкция" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Служебная информация" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
   <si>
     <t xml:space="preserve">Общие</t>
   </si>
@@ -489,6 +490,24 @@
   </si>
   <si>
     <t xml:space="preserve">Персональные данные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Версия R7.University:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{UniversityVersion}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Данные выгружены:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{DataExportedAtDateTime}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пользователь, выгрузивший данные:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{DataExportedByUserName}}</t>
   </si>
 </sst>
 </file>
@@ -616,7 +635,7 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1252,4 +1271,57 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add tests project for Core library
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -99,6 +99,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Повышение квалификации,
 Профессиональная переподготовка, сертификация, стажировка и др.
@@ -239,7 +240,7 @@
     <t xml:space="preserve">Или ссылка на eLibrary.ru:</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.elibrary.ru/author_items.asp?authorid={{ScienceIndexAuthorId}}</t>
+    <t xml:space="preserve">https://www.elibrary.ru/author_items.asp?authorid={{ScienceIndexAuthorId}}&amp;firstname={{FirstName}}</t>
   </si>
   <si>
     <t xml:space="preserve">Рабочее место и график работы</t>
@@ -575,6 +576,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -625,7 +627,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -650,23 +652,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -753,10 +743,10 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topRight" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,7 +992,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="B3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
@@ -1016,12 +1006,12 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1092,12 +1082,12 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1179,8 +1169,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.1"/>
@@ -1188,7 +1178,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1273,16 +1263,16 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1380,13 +1370,13 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1411,16 +1401,16 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>95</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1459,7 +1449,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1484,7 +1474,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="5" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1509,7 +1499,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="5" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1524,7 +1514,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1557,7 +1547,7 @@
       <c r="A23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="5" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1577,7 +1567,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="5" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1612,7 +1602,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="36.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="36.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
Fix value localization in template, fix wrong tag for WorkingHours, some minor template tweaks GH-305
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -498,7 +498,7 @@
     <t xml:space="preserve">Рабочий график:</t>
   </si>
   <si>
-    <t xml:space="preserve">{{WorkSchedule}}</t>
+    <t xml:space="preserve">{{WorkingHours}}</t>
   </si>
   <si>
     <t xml:space="preserve">Стаж работы</t>
@@ -964,6 +964,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1145,13 +1146,13 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B9" activeCellId="1" sqref="A64:A65 B9"/>
+      <selection pane="topRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.17"/>
@@ -1392,7 +1393,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B15" activeCellId="1" sqref="A64:A65 B15"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1486,7 +1487,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="A64:A65 A5"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1495,7 +1496,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -1597,15 +1598,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="1" sqref="A64:A65 D21"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="83.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
@@ -1706,7 +1707,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="B3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D33" activeCellId="1" sqref="A64:A65 D33"/>
+      <selection pane="bottomLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1716,7 +1717,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="57.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -1856,7 +1857,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="1" sqref="A64:A65 B17"/>
+      <selection pane="bottomLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1952,8 +1953,8 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A64:A65 A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1967,7 +1968,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="135.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>117</v>
       </c>
@@ -2010,8 +2011,8 @@
   </sheetPr>
   <dimension ref="A1:A58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A64:A65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2297,7 +2298,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B30" activeCellId="1" sqref="A64:A65 B30"/>
+      <selection pane="topRight" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Don't explicitly render "No" state for primary positions and title achievements, minor template changes GH-305
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -186,6 +186,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Да/нет</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -235,6 +248,18 @@
         </r>
       </text>
     </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">НЕ обязательно! Для новых или обновляемых документов — имя файла.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -274,16 +299,15 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">НЕ обязательно!</t>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">НЕ обязательно! Для новых или обновляемых документов — имя файла.</t>
         </r>
       </text>
     </comment>
@@ -302,12 +326,23 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Титульные достижения обычно отображаются вместе с именем, например, «профессор Иванов И.И.»
-</t>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Да/нет. Титульные достижения обычно отображаются вместе с именем, например, «профессор Иванов И.И.»</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">НЕ обязательно! Для новых или обновляемых документов — имя файла.</t>
         </r>
       </text>
     </comment>
@@ -525,7 +560,7 @@
     <t xml:space="preserve">Подразделение</t>
   </si>
   <si>
-    <t xml:space="preserve">Основная должность (да/нет)</t>
+    <t xml:space="preserve">Основная должность?</t>
   </si>
   <si>
     <t xml:space="preserve">{% for position in Positions %}</t>
@@ -573,7 +608,7 @@
     <t xml:space="preserve">Описание</t>
   </si>
   <si>
-    <t xml:space="preserve">Ссылка на документ (или имя файла для новых документов)</t>
+    <t xml:space="preserve">Ссылка на документ</t>
   </si>
   <si>
     <t xml:space="preserve">{% for education in Education %}</t>
@@ -648,7 +683,7 @@
     <t xml:space="preserve">Дополнение наименования</t>
   </si>
   <si>
-    <t xml:space="preserve">Титульное (да/нет)</t>
+    <t xml:space="preserve">Титульное?</t>
   </si>
   <si>
     <t xml:space="preserve">{% for achievement in Achievements %}</t>
@@ -916,7 +951,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -954,10 +989,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1059,7 +1105,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1143,10 +1189,10 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1393,7 +1439,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1484,10 +1530,10 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1496,7 +1542,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.1"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -1598,7 +1644,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1707,7 +1753,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="B3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1953,7 +1999,7 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Convert About HTML to Markdown on export GH-305
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,6 +255,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">НЕ обязательно! Для новых или обновляемых документов — имя файла.</t>
         </r>
@@ -306,6 +307,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">НЕ обязательно! Для новых или обновляемых документов — имя файла.</t>
         </r>
@@ -329,6 +331,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Да/нет. Титульные достижения обычно отображаются вместе с именем, например, «профессор Иванов И.И.»</t>
         </r>
@@ -341,6 +344,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">НЕ обязательно! Для новых или обновляемых документов — имя файла.</t>
         </r>
@@ -414,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="178">
   <si>
     <t xml:space="preserve">Фамилия:</t>
   </si>
@@ -776,7 +780,13 @@
     <t xml:space="preserve">- НЕ следует дублировать здесь сведения, приведенные в других разделах.</t>
   </si>
   <si>
-    <t xml:space="preserve">- Данный текст может содержать ссылки на внешние ресурсы и минимальное форматирование (выделение, списки).</t>
+    <t xml:space="preserve">- Поле "О себе" в формах, загруженных с сайта, содержит упрощенное текстовое представление информации, размещенной на сайте.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- При правке информации в поле "О себе" допускается использовать элементы языка разметки Markdown:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ru.wikipedia.org/wiki/Markdown</t>
   </si>
   <si>
     <t xml:space="preserve">Порядок внесения изменений в сведения о сотруднике на сайте</t>
@@ -951,7 +961,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -989,11 +999,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1001,7 +1006,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1064,7 +1069,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1105,7 +1110,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1189,7 +1198,7 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
@@ -1997,16 +2006,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="193.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="136.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="91.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,9 +2025,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="135.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="0" t="s">
         <v>117</v>
       </c>
+      <c r="B2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
@@ -2039,7 +2053,20 @@
         <v>120</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1" display="https://ru.wikipedia.org/wiki/Markdown"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2069,157 +2096,157 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,97 +2254,97 @@
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
-        <v>169</v>
+      <c r="A58" s="11" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2356,26 +2383,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update instruction in the template GH-305
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="173">
   <si>
     <t xml:space="preserve">Фамилия:</t>
   </si>
@@ -792,19 +792,13 @@
     <t xml:space="preserve">Порядок внесения изменений в сведения о сотруднике на сайте</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Войти на сайт под своей учетной записью, при необходимости зарегистрироваться на сайте.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Открыть карточку сотрудника на сайте, нажать кнопку «Экспорт в .XLSX».</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Скачать заполненную форму в виде файла формата .XLSX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Произвести необходимые правки таким образом, чтобы новое состояние формы в полной мере отражало текущее (актуальное) состояние дел.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Оформить заявку на размещение/обновление информации на сайте, отправить материалы руководителю проекта по созданию сайта (администратору сайта). </t>
+    <t xml:space="preserve">1. Открыть карточку сотрудника на сайте, нажать кнопку «Экспортировать», пройти проверку «Я не робот» и скачать заполненную форму в виде файла формата .XLSX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Произвести необходимые правки таким образом, чтобы новое состояние формы в полной мере отражало текущее (актуальное) состояние дел.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Сформировать заявку на размещение/обновление информации на сайте, отправить материалы руководителю проекта по созданию сайта (администратору сайта). </t>
   </si>
   <si>
     <t xml:space="preserve">Общие правила и замечания</t>
@@ -813,16 +807,7 @@
     <t xml:space="preserve">- При необходимости внесения изменений в сведения о сотруднике на сайте, всегда сначала скачивайте форму из карточки на сайте!</t>
   </si>
   <si>
-    <t xml:space="preserve">- Скачивание форм сотрудников в настоящее время доступно всем зарегистрированным пользователям сайта.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Регистрация на сайте осуществляется самостоятельно, с подтверждением адреса Email. Если письмо со ссылкой для подтверждения регистрации не приходит, проверьте папку "Спам".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Для получения актуальной версии своей формы вы также можете обратиться к зам. декана по информатизации своего факультета. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Если информация о сотруднике была ранее размещена на сайте, но теперь не доступна, для получения заполненной формы обратитесь к администратору сайта.</t>
+    <t xml:space="preserve">- Если известно, что информация о сотруднике была ранее размещена на сайте, но более не доступна, для получения заполненной формы обратитесь к администратору сайта.</t>
   </si>
   <si>
     <t xml:space="preserve">Заполнение формы</t>
@@ -961,7 +946,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1003,12 +988,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1069,7 +1048,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1111,10 +1090,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2008,7 +1983,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -2082,10 +2057,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2114,98 +2089,98 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="0" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2220,136 +2195,111 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="48" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A58" r:id="rId1" display="https://github.com/roman-yagodin/R7.University/issues/new"/>
+    <hyperlink ref="A53" r:id="rId1" display="https://github.com/roman-yagodin/R7.University/issues/new"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2383,26 +2333,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Template should open on the first sheet
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -1173,7 +1173,7 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
@@ -2059,7 +2059,7 @@
   </sheetPr>
   <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update instruction in template, save template with LibreOffice 6
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A6" authorId="0">
@@ -157,7 +157,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -206,7 +206,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -268,7 +268,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -320,7 +320,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="E2" authorId="0">
@@ -357,7 +357,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -395,7 +395,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Бакалавриат, Бакалавриат академический, Бакалавриат прикладной, Магистратура, Магистратура академическая, Магистратура прикладная, Специалитет, Специалитет СПО (на базе 9 кл.), Специалитет СПО (на базе 11 кл.)</t>
+          <t xml:space="preserve">Возможные значения: Бакалавриат, Бакалавриат академический, Бакалавриат прикладной, Магистратура, Магистратура академическая, Магистратура прикладная, Специалитет, Специалитет СПО (на базе 9 кл.), Специалитет СПО (на базе 11 кл.)</t>
         </r>
       </text>
     </comment>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="174">
   <si>
     <t xml:space="preserve">Фамилия:</t>
   </si>
@@ -765,7 +765,10 @@
     <t xml:space="preserve">- Раздел заполняется только преподавателями, обязателен к заполнению!</t>
   </si>
   <si>
-    <t xml:space="preserve">- Таблица должна отражать полный актуальный перечень преподаваемых дисциплин на текущий учебный год!</t>
+    <t xml:space="preserve">- Таблица должна отражать полный актуальный перечень преподаваемых дисциплин на текущий учебный год.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- НЕ указывайте более одного названия образовательной программы, профиля, уровня образования на строку - при необходимости, продублируйте строку ниже!</t>
   </si>
   <si>
     <t xml:space="preserve">О себе</t>
@@ -1095,13 +1098,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1173,13 +1176,13 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.94"/>
@@ -1426,7 +1429,7 @@
       <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.2"/>
@@ -1520,7 +1523,7 @@
       <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.56"/>
@@ -1631,7 +1634,7 @@
       <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
@@ -1740,7 +1743,7 @@
       <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.92"/>
@@ -1882,15 +1885,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.57"/>
@@ -1962,6 +1965,11 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1987,7 +1995,7 @@
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="136.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="91.15"/>
@@ -1996,12 +2004,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="135.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B2" s="9"/>
     </row>
@@ -2015,27 +2023,27 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2063,7 +2071,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="238.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
@@ -2071,132 +2079,132 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,97 +2212,97 @@
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2324,7 +2332,7 @@
       <selection pane="topRight" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="43.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.64"/>
@@ -2333,26 +2341,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update instructions in the template
</commit_message>
<xml_diff>
--- a/R7.University/assets/templates/employee_template.xlsx
+++ b/R7.University/assets/templates/employee_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Общие сведения" sheetId="1" state="visible" r:id="rId2"/>
@@ -795,13 +795,13 @@
     <t xml:space="preserve">Порядок внесения изменений в сведения о сотруднике на сайте</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Открыть карточку сотрудника на сайте, нажать кнопку «Экспортировать», пройти проверку «Я не робот» и скачать заполненную форму в виде файла формата .XLSX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Произвести необходимые правки таким образом, чтобы новое состояние формы в полной мере отражало текущее (актуальное) состояние дел.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Сформировать заявку на размещение/обновление информации на сайте, отправить материалы руководителю проекта по созданию сайта (администратору сайта). </t>
+    <t xml:space="preserve">1. Откройте карточку сотрудника на сайте, нажмите кнопку "Экспорт сведений", пройдите проверку "Я не робот" и скачайте заполненную форму в виде файла формата .XLSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Произведите необходимые правки таким образом, чтобы новое состояние формы в полной мере отражало текущее (актуальное) состояние дел.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Сформируйте заявку на размещение/обновление информации на сайте и отправьте материалы руководителю проекта по созданию сайта (администратору сайта).</t>
   </si>
   <si>
     <t xml:space="preserve">Общие правила и замечания</t>
@@ -810,7 +810,23 @@
     <t xml:space="preserve">- При необходимости внесения изменений в сведения о сотруднике на сайте, всегда сначала скачивайте форму из карточки на сайте!</t>
   </si>
   <si>
-    <t xml:space="preserve">- Если известно, что информация о сотруднике была ранее размещена на сайте, но более не доступна, для получения заполненной формы обратитесь к администратору сайта.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Если сведения о сотруднике не удается найти на сайте, но Вы уверены, что сведения о нем ранее были опубликованы на сайте, обратитесь к руководителю проекта по созданию сайта (администратору сайта).</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Заполнение формы</t>
@@ -949,7 +965,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -998,6 +1014,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1887,10 +1908,10 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2067,8 +2088,8 @@
   </sheetPr>
   <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>